<commit_message>
First attempt to integrate the optocouplers with the main PCB.
</commit_message>
<xml_diff>
--- a/PCB/BOM.xlsx
+++ b/PCB/BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\Desktop\Autotuning github\Versión 2\PCB impedance matching\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\AUTOTUNING\AutotuningReleMosfetArduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F42ABE7-3F6E-462B-830A-3BAC3577B9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88B3AA9-58EC-4947-9890-252896C9BF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{015E6577-A28D-4182-9722-EB61EDAAFD6B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
   <si>
     <t>References</t>
   </si>
@@ -113,12 +113,30 @@
     <t>resistencia 1.2k</t>
   </si>
   <si>
+    <t>resistencia 3.9k</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3.9k</t>
+  </si>
+  <si>
     <t>100k</t>
   </si>
   <si>
+    <t>MBA02040C3901FCT00</t>
+  </si>
+  <si>
     <t>SFR2500001003JA500</t>
   </si>
   <si>
+    <t>optoacoplador</t>
+  </si>
+  <si>
+    <t>OPT_S1…S5,OPTM1..M5,OPT_T1…T5,OPT_TTL</t>
+  </si>
+  <si>
+    <t>EL817</t>
+  </si>
+  <si>
     <t>SMA a Panel</t>
   </si>
   <si>
@@ -152,7 +170,13 @@
     <t>DSRL1..5,DTRL1..5,DMRL1..5,DTTL5</t>
   </si>
   <si>
+    <t>no montar</t>
+  </si>
+  <si>
     <t>observaciones</t>
+  </si>
+  <si>
+    <t>Esta hecho con espejp, por lo tando van montado por la parte posterior(Bottom)</t>
   </si>
   <si>
     <t>jumper hembra</t>
@@ -246,7 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -255,7 +279,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -272,6 +301,232 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>68036</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>611958</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>48986</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="Grupo 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C66C85F3-B806-1F7C-FB50-18344097FFCC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="0" y="2735036"/>
+          <a:ext cx="10552594" cy="6648450"/>
+          <a:chOff x="427628" y="66264"/>
+          <a:chExt cx="10545172" cy="6648450"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="5" name="Imagen 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EEF9D22-ADE5-8A94-7464-178663AC9E4F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="427628" y="143285"/>
+            <a:ext cx="2753182" cy="6571429"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="6" name="Imagen 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AD4F244-A9A2-CEC9-8335-9BC916108478}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3316082" y="66264"/>
+            <a:ext cx="2905125" cy="6648450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="CuadroTexto 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41FC6CE9-8AC3-C763-CB75-13E2F5018C75}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6459794" y="486697"/>
+            <a:ext cx="4513006" cy="923330"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="es-ES"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>La representación en 3d está mal, deberían aparecer abajo porque hay un espejo hecho en la PCB (2D), pero el CAD no lo muestra</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -591,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DCDBD2-A7F2-436E-9545-795CA809C7F8}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,8 +878,8 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>38</v>
+      <c r="F1" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -665,10 +920,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -706,7 +961,7 @@
       <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -740,10 +995,10 @@
         <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>21</v>
@@ -758,74 +1013,156 @@
         <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E9" s="2">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E10" s="2">
-        <v>11</v>
-      </c>
-      <c r="F10" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="D11" s="4" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2">
-        <v>16</v>
-      </c>
-      <c r="F11" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2">
+        <v>17</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="B13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="2">
+      <c r="D13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2">
+        <v>48</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="2">
         <v>16</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="F14" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -835,12 +1172,15 @@
     <hyperlink ref="D5" r:id="rId4" xr:uid="{330BE76A-CE75-4E47-9884-CC47DE4AD207}"/>
     <hyperlink ref="D6" r:id="rId5" xr:uid="{5BEF3131-272E-441D-9E7E-D01FC9295CA9}"/>
     <hyperlink ref="D7" r:id="rId6" xr:uid="{3702BA69-16CD-4BD8-A046-F2B599A350D5}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{4EB4BE1C-2BBE-46E7-8713-4F4E5CB2B0EF}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{D264D66A-591E-4092-9A79-89BF100B2D52}"/>
-    <hyperlink ref="D10" r:id="rId9" xr:uid="{1F22BB7C-09C9-403F-8B32-DC3767E0B58C}"/>
-    <hyperlink ref="D11" r:id="rId10" xr:uid="{E8F8B395-3030-4B25-A602-DAB882379BCC}"/>
-    <hyperlink ref="D12" r:id="rId11" xr:uid="{3BC2536E-6269-48B4-8A06-362D22060AF1}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{6D0F23A6-A638-4D43-9793-D2AC53E68F16}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{4EB4BE1C-2BBE-46E7-8713-4F4E5CB2B0EF}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{6F956BDA-14A3-4216-B76F-91345A162C72}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{D264D66A-591E-4092-9A79-89BF100B2D52}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{1F22BB7C-09C9-403F-8B32-DC3767E0B58C}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{E8F8B395-3030-4B25-A602-DAB882379BCC}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{3BC2536E-6269-48B4-8A06-362D22060AF1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BOM modification for optocoupler compatibility
</commit_message>
<xml_diff>
--- a/PCB/BOM.xlsx
+++ b/PCB/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\Desktop\Autotuning github\Versión 2\PCB impedance matching\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\serverphysiomri\6. FABRICACIÓN2\Proyecto Ymir\3. Autotuning\Gerber\Gerber Autotuning V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F42ABE7-3F6E-462B-830A-3BAC3577B9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB5A7DC-39DF-4775-9749-1DDF93BD7E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{015E6577-A28D-4182-9722-EB61EDAAFD6B}"/>
+    <workbookView xWindow="-120" yWindow="240" windowWidth="29040" windowHeight="16080" xr2:uid="{015E6577-A28D-4182-9722-EB61EDAAFD6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t>References</t>
   </si>
@@ -44,9 +42,6 @@
     <t>Part number</t>
   </si>
   <si>
-    <t>link</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -83,24 +78,6 @@
     <t>Descripción</t>
   </si>
   <si>
-    <t>rele</t>
-  </si>
-  <si>
-    <t>mosfet</t>
-  </si>
-  <si>
-    <t>diodo</t>
-  </si>
-  <si>
-    <t>resistencia 10k</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>SFR2500001002FA500</t>
-  </si>
-  <si>
     <t>digikey</t>
   </si>
   <si>
@@ -110,36 +87,18 @@
     <t>1.2k</t>
   </si>
   <si>
-    <t>resistencia 1.2k</t>
-  </si>
-  <si>
     <t>100k</t>
   </si>
   <si>
     <t>SFR2500001003JA500</t>
   </si>
   <si>
-    <t>SMA a Panel</t>
-  </si>
-  <si>
-    <t>CETRONIC</t>
-  </si>
-  <si>
-    <t>CONECTOR SMA HEMBRA A PANEL</t>
-  </si>
-  <si>
-    <t>PMW S1..5, PMW T1..5, PMW M1..5, COIL, AMPLI, VNA</t>
-  </si>
-  <si>
     <t>691213710002</t>
   </si>
   <si>
     <t>PMW S1..5, PMW T1..5, PMW M1..5, COIL, GND, 5V</t>
   </si>
   <si>
-    <t>Borne para PCB Hembra</t>
-  </si>
-  <si>
     <t>J1-J16</t>
   </si>
   <si>
@@ -152,29 +111,83 @@
     <t>DSRL1..5,DTRL1..5,DMRL1..5,DTTL5</t>
   </si>
   <si>
-    <t>observaciones</t>
-  </si>
-  <si>
-    <t>jumper hembra</t>
-  </si>
-  <si>
-    <t>jumper Macho</t>
-  </si>
-  <si>
     <t>AKSCT/Z BLACK</t>
   </si>
   <si>
     <t>rs</t>
   </si>
   <si>
-    <t>Aereo</t>
+    <t xml:space="preserve">SMA PCB </t>
+  </si>
+  <si>
+    <t>Terminal regleta PCB</t>
+  </si>
+  <si>
+    <t>Resistencia 100k</t>
+  </si>
+  <si>
+    <t>Resistencia 1.2k</t>
+  </si>
+  <si>
+    <t>EC - 0034</t>
+  </si>
+  <si>
+    <t>EC - 0033</t>
+  </si>
+  <si>
+    <t>EC - 0035</t>
+  </si>
+  <si>
+    <t>EC - 0048</t>
+  </si>
+  <si>
+    <t>Rele</t>
+  </si>
+  <si>
+    <t>Mosfet</t>
+  </si>
+  <si>
+    <t>Jumper Macho</t>
+  </si>
+  <si>
+    <t>Diodo</t>
+  </si>
+  <si>
+    <t>Jumper hembra</t>
+  </si>
+  <si>
+    <t>EC - 0026</t>
+  </si>
+  <si>
+    <t>EC - 0038</t>
+  </si>
+  <si>
+    <t>Se ponen en el mismo lugar que los Jumper hembra (EC - 0026)</t>
+  </si>
+  <si>
+    <t>EC - 0031</t>
+  </si>
+  <si>
+    <t>RF - 0007</t>
+  </si>
+  <si>
+    <t>EC - 0039</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>901-144-8RFX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,7 +259,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -256,6 +269,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -591,25 +609,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DCDBD2-A7F2-436E-9545-795CA809C7F8}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="73.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -618,213 +636,211 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2">
         <v>16</v>
       </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2">
         <v>16</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="E4" s="2">
         <v>16</v>
       </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="E5" s="2">
         <v>32</v>
       </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2">
         <v>16</v>
       </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="2">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="D9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="2">
+        <v>16</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="2">
+      <c r="C10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="2">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="D11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="2">
-        <v>16</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="E11" s="7">
         <v>3</v>
       </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="2">
-        <v>11</v>
-      </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="2">
-        <v>16</v>
-      </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="2">
-        <v>16</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>43</v>
+      <c r="F11" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -833,13 +849,12 @@
     <hyperlink ref="D3" r:id="rId2" xr:uid="{152D71E1-7945-446A-9D34-57882B900AA2}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{9625E330-E31F-416E-BD89-6D85104DE4C1}"/>
     <hyperlink ref="D5" r:id="rId4" xr:uid="{330BE76A-CE75-4E47-9884-CC47DE4AD207}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{5BEF3131-272E-441D-9E7E-D01FC9295CA9}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{3702BA69-16CD-4BD8-A046-F2B599A350D5}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{4EB4BE1C-2BBE-46E7-8713-4F4E5CB2B0EF}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{D264D66A-591E-4092-9A79-89BF100B2D52}"/>
-    <hyperlink ref="D10" r:id="rId9" xr:uid="{1F22BB7C-09C9-403F-8B32-DC3767E0B58C}"/>
-    <hyperlink ref="D11" r:id="rId10" xr:uid="{E8F8B395-3030-4B25-A602-DAB882379BCC}"/>
-    <hyperlink ref="D12" r:id="rId11" xr:uid="{3BC2536E-6269-48B4-8A06-362D22060AF1}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{3702BA69-16CD-4BD8-A046-F2B599A350D5}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{4EB4BE1C-2BBE-46E7-8713-4F4E5CB2B0EF}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{1F22BB7C-09C9-403F-8B32-DC3767E0B58C}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{E8F8B395-3030-4B25-A602-DAB882379BCC}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{3BC2536E-6269-48B4-8A06-362D22060AF1}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{EB4FEB25-C9E4-4C3C-AA05-95FE11A3AB4E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>